<commit_message>
teams public page filtered accordingly
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="72">
   <si>
     <t xml:space="preserve">Team Name</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t xml:space="preserve">Team13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X Team13</t>
   </si>
 </sst>
 </file>
@@ -359,7 +365,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -858,6 +864,88 @@
         <v>18</v>
       </c>
       <c r="M12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1876,6 +1964,10 @@
     <hyperlink ref="H11" r:id="rId30" display="safwan.du16@gmail.com"/>
     <hyperlink ref="F12" r:id="rId31" display="jecile7288@netjook.com"/>
     <hyperlink ref="H12" r:id="rId32" display="safwan.du16@gmail.com"/>
+    <hyperlink ref="F13" r:id="rId33" display="jecile7288@netjook.com"/>
+    <hyperlink ref="H13" r:id="rId34" display="safwan.du16@gmail.com"/>
+    <hyperlink ref="F14" r:id="rId35" display="jecile7288@netjook.com"/>
+    <hyperlink ref="H14" r:id="rId36" display="safwan.du16@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>